<commit_message>
Completed SB testing in zeus in tick#18
</commit_message>
<xml_diff>
--- a/App_Release/Zeus_FW_SB430_3110_SS501_SC206.xlsx
+++ b/App_Release/Zeus_FW_SB430_3110_SS501_SC206.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\001-Github\RYSE_Testing_record\App_Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E313AAC-CB4D-47F0-A9C4-4A47DAD8551C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA477D76-0C13-459C-BE94-4A3C672E2DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="166">
   <si>
     <t>Code</t>
   </si>
@@ -531,6 +531,42 @@
   </si>
   <si>
     <t>Valid ChangeTimezone</t>
+  </si>
+  <si>
+    <t>26-03-2025</t>
+  </si>
+  <si>
+    <t>Encoder position read error caused by removing the wrong device (Zeus). It's fine</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Bridge_Part1_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Bridge_Part2_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Bridge_Part3_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Group_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Routine_Part1_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Routine_Part2_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Routine_Part3_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Routine_Part4_26Mar2024</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_Routine_Part5_26Mar2024</t>
+  </si>
+  <si>
+    <t>Morning and afternoon routine create and check fail but fine~</t>
   </si>
 </sst>
 </file>
@@ -693,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -717,9 +753,6 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -727,11 +760,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="190">
+  <dxfs count="15">
     <dxf>
       <font>
         <b/>
@@ -842,1319 +879,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3D2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8DBFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFCBF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFCBF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFCBF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2504,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA5EB23-85E7-4EC6-9FFB-9E2F32772CB4}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82:D83"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2518,13 +1242,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="17" t="s">
         <v>113</v>
       </c>
@@ -2557,11 +1281,11 @@
         <v>9</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="11"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -2569,11 +1293,11 @@
         <v>94</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="28"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>87</v>
       </c>
@@ -2581,11 +1305,11 @@
         <v>95</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="29"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>88</v>
       </c>
@@ -2593,11 +1317,11 @@
         <v>96</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="28"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>89</v>
       </c>
@@ -2605,11 +1329,11 @@
         <v>97</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="29"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>90</v>
       </c>
@@ -2617,11 +1341,11 @@
         <v>98</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="28"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>91</v>
       </c>
@@ -2629,11 +1353,11 @@
         <v>100</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="29"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>92</v>
       </c>
@@ -2641,11 +1365,11 @@
         <v>99</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="28"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>93</v>
       </c>
@@ -2653,7 +1377,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="29"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
@@ -2667,8 +1391,12 @@
       <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
@@ -2679,9 +1407,15 @@
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2691,9 +1425,15 @@
       <c r="B15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>156</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="10"/>
     </row>
@@ -2704,9 +1444,15 @@
       <c r="B16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1"/>
     </row>
@@ -2717,8 +1463,10 @@
       <c r="B17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="28"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="10"/>
@@ -2730,9 +1478,15 @@
       <c r="B18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1"/>
     </row>
@@ -2743,9 +1497,15 @@
       <c r="B19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>157</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="10"/>
     </row>
@@ -2756,9 +1516,15 @@
       <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="1"/>
     </row>
@@ -2769,9 +1535,15 @@
       <c r="B21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="10"/>
     </row>
@@ -2782,9 +1554,15 @@
       <c r="B22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="1"/>
     </row>
@@ -2803,7 +1581,7 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
@@ -2811,12 +1589,12 @@
         <v>105</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="28"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>103</v>
       </c>
@@ -2824,12 +1602,12 @@
         <v>106</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="29"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>104</v>
       </c>
@@ -2837,7 +1615,7 @@
         <v>107</v>
       </c>
       <c r="C27" s="20"/>
-      <c r="D27" s="30"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="10"/>
@@ -3083,16 +1861,16 @@
       <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
@@ -3165,9 +1943,15 @@
       <c r="B58" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+      <c r="C58" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3177,9 +1961,15 @@
       <c r="B59" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="C59" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3189,9 +1979,15 @@
       <c r="B60" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
+      <c r="C60" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -3201,9 +1997,15 @@
       <c r="B61" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="C61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3213,9 +2015,15 @@
       <c r="B62" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
+      <c r="C62" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -3225,10 +2033,18 @@
       <c r="B63" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="C63" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="64" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -3251,8 +2067,12 @@
         <v>111</v>
       </c>
       <c r="C66" s="3"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3273,8 +2093,12 @@
         <v>83</v>
       </c>
       <c r="C68" s="20"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
+      <c r="D68" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>160</v>
+      </c>
       <c r="F68" s="19"/>
     </row>
     <row r="69" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3285,21 +2109,29 @@
         <v>84</v>
       </c>
       <c r="C69" s="8"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
+      <c r="D69" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="F69" s="7"/>
     </row>
     <row r="70" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="26" t="s">
+      <c r="A70" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B70" s="26" t="s">
+      <c r="B70" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C70" s="27"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="F70" s="25"/>
     </row>
     <row r="71" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
@@ -3309,8 +2141,12 @@
         <v>150</v>
       </c>
       <c r="C71" s="8"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
+      <c r="D71" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="F71" s="7"/>
     </row>
     <row r="72" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3321,6 +2157,12 @@
         <v>151</v>
       </c>
       <c r="C72" s="20"/>
+      <c r="D72" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="73" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
@@ -3330,9 +2172,15 @@
         <v>152</v>
       </c>
       <c r="C73" s="8"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
+      <c r="D73" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="74" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="19" t="s">
@@ -3342,6 +2190,9 @@
         <v>153</v>
       </c>
       <c r="C74" s="20"/>
+      <c r="E74" s="19" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="75" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -3413,7 +2264,7 @@
         <v>75</v>
       </c>
       <c r="C82" s="3"/>
-      <c r="D82" s="30"/>
+      <c r="D82" s="29"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
@@ -3425,7 +2276,7 @@
         <v>76</v>
       </c>
       <c r="C83" s="8"/>
-      <c r="D83" s="29"/>
+      <c r="D83" s="28"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
     </row>
@@ -3489,14 +2340,6 @@
       <formula>NOT(ISERROR(SEARCH("AX0",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D87:D1048576 D1:D84">
-    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B1:F1048576">
     <cfRule type="dataBar" priority="1">
       <dataBar>
@@ -3509,6 +2352,14 @@
           <x14:id>{3E9BFF79-6FA6-4436-8241-E21D739BAB05}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D1048576 D1:D84">
+    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>